<commit_message>
tiva ADC values table formatted
</commit_message>
<xml_diff>
--- a/tivaADCvalues.xlsx
+++ b/tivaADCvalues.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxwe\Documents\GitHub\Bms_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62A60AB-21EA-458D-BCCE-9EF78B5459C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAF3C68-E0AD-4BCD-8757-27DEF80D9218}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{F5A83452-C2F1-40C1-8D19-958A390814ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="tivaADCvalues" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -138,20 +138,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,124 +490,124 @@
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8"/>
+      <c r="B2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="10"/>
       <c r="B3" s="4">
         <v>2.7</v>
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="8"/>
+    <row r="4" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="10"/>
       <c r="B4" s="4">
         <v>2.8</v>
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8"/>
+    <row r="5" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="10"/>
       <c r="B5" s="4">
         <v>2.9</v>
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="8"/>
+    <row r="6" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="10"/>
       <c r="B6" s="4">
         <v>3</v>
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="8"/>
+    <row r="7" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="10"/>
       <c r="B7" s="4">
         <v>3.1</v>
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="8"/>
+    <row r="8" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="10"/>
       <c r="B8" s="4">
         <v>3.2</v>
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="8"/>
+    <row r="9" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="10"/>
       <c r="B9" s="4">
         <v>3.3</v>
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="8"/>
+    <row r="10" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="10"/>
       <c r="B10" s="4">
         <v>3.4</v>
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="8"/>
+    <row r="11" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="10"/>
       <c r="B11" s="4">
         <v>3.5</v>
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="8"/>
+    <row r="12" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="10"/>
       <c r="B12" s="4">
         <v>3.6</v>
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="8"/>
+    <row r="13" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="10"/>
       <c r="B13" s="4">
         <v>3.7</v>
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="8"/>
+    <row r="14" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="10"/>
       <c r="B14" s="4">
         <v>3.8</v>
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="8"/>
+    <row r="15" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="10"/>
       <c r="B15" s="4">
         <v>3.9</v>
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="8"/>
+    <row r="16" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="10"/>
       <c r="B16" s="4">
         <v>4</v>
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="8"/>
+    <row r="17" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="10"/>
       <c r="B17" s="4">
         <v>4.0999999999999996</v>
       </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="10"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="3">
         <v>4.1999999999999904</v>
       </c>

</xml_diff>